<commit_message>
updated to fix bugs related to auto mode
</commit_message>
<xml_diff>
--- a/robots/claymore/AutoModesAnalysis.xlsx
+++ b/robots/claymore/AutoModesAnalysis.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\robotics\robotdev\robots\claymore\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\ButchGriffin\src\robotdev\robots\claymore\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17740" xr2:uid="{3E3E0330-88BD-4F34-939F-40E93F24D94C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17736" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="c_switch_r" sheetId="2" r:id="rId2"/>
+    <sheet name="c_switch_l" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
   <si>
     <t>Number</t>
   </si>
@@ -81,12 +83,24 @@
   </si>
   <si>
     <t>Right Switch Back</t>
+  </si>
+  <si>
+    <t>Attempt</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Time (s)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -130,10 +144,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,23 +465,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFCCE82E-CFC4-426F-8696-8C1FFFDEC1DA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" customWidth="1"/>
-    <col min="3" max="3" width="27.7265625" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27.77734375" customWidth="1"/>
+    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,7 +498,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -502,7 +519,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -519,7 +536,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -536,7 +553,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -548,7 +565,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -565,7 +582,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -577,7 +594,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -594,7 +611,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -606,7 +623,7 @@
       </c>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -623,7 +640,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -635,44 +652,316 @@
       </c>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D24" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>2.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>7.3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated to tweak auto modes, fixed the eject step to provide more flexibility
</commit_message>
<xml_diff>
--- a/robots/claymore/AutoModesAnalysis.xlsx
+++ b/robots/claymore/AutoModesAnalysis.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17736" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17736" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="c_switch_r" sheetId="2" r:id="rId2"/>
     <sheet name="c_switch_l" sheetId="3" r:id="rId3"/>
+    <sheet name="r_scale_r" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="23">
   <si>
     <t>Number</t>
   </si>
@@ -836,6 +837,142 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>7.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
@@ -861,7 +998,7 @@
         <v>21</v>
       </c>
       <c r="C2">
-        <v>7.2</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -872,7 +1009,7 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>7.2</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -883,7 +1020,7 @@
         <v>21</v>
       </c>
       <c r="C4">
-        <v>7.2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -894,7 +1031,7 @@
         <v>21</v>
       </c>
       <c r="C5">
-        <v>7.2</v>
+        <v>7.51</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -905,7 +1042,7 @@
         <v>21</v>
       </c>
       <c r="C6">
-        <v>8.1999999999999993</v>
+        <v>7.61</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -916,7 +1053,7 @@
         <v>21</v>
       </c>
       <c r="C7">
-        <v>8.1999999999999993</v>
+        <v>7.67</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -927,7 +1064,7 @@
         <v>21</v>
       </c>
       <c r="C8">
-        <v>7.9</v>
+        <v>7.67</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -938,7 +1075,7 @@
         <v>21</v>
       </c>
       <c r="C9">
-        <v>7.3</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -949,7 +1086,7 @@
         <v>21</v>
       </c>
       <c r="C10">
-        <v>7.3</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -960,7 +1097,7 @@
         <v>21</v>
       </c>
       <c r="C11">
-        <v>7.3</v>
+        <v>7.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>